<commit_message>
support filter  in index checker
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D113A64-801C-B641-8352-68D3B181828A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15740A5-6BED-40C9-84BB-8D7348EFD417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-15" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1873,12 +1873,6 @@
     <t>value &gt; 0 &amp;&amp; value &lt; 20</t>
   </si>
   <si>
-    <t>id=item#*.id</t>
-  </si>
-  <si>
-    <t>id=item#item.id</t>
-  </si>
-  <si>
     <t>[1]</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1888,6 +1882,14 @@
   </si>
   <si>
     <t>@config</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>id==item#item.id</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>id==item#*.id</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1895,11 +1897,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1928,7 +1930,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1948,7 +1950,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2234,7 +2236,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="常规 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
@@ -3161,23 +3163,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="45.875" customWidth="1"/>
+    <col min="6" max="6" width="18.625" customWidth="1"/>
+    <col min="8" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3185,7 +3187,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
     </row>
-    <row r="2" spans="1:9" ht="16">
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3214,7 +3216,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16">
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3243,7 +3245,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16">
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3258,7 +3260,7 @@
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3287,7 +3289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16">
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -3304,7 +3306,7 @@
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="16">
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>17</v>
       </c>
@@ -3333,7 +3335,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16">
+    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -3356,7 +3358,7 @@
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:9" ht="16">
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
@@ -3379,7 +3381,7 @@
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
     </row>
-    <row r="10" spans="1:9" ht="16">
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
         <v>17</v>
       </c>
@@ -3402,7 +3404,7 @@
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:9" ht="16">
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
@@ -3425,7 +3427,7 @@
       <c r="H11" s="35"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="12" spans="1:9" ht="16">
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>17</v>
       </c>
@@ -3448,7 +3450,7 @@
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:9" ht="16">
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>17</v>
       </c>
@@ -3471,7 +3473,7 @@
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
     </row>
-    <row r="14" spans="1:9" ht="16">
+    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>17</v>
       </c>
@@ -3498,7 +3500,7 @@
       </c>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:9" ht="16">
+    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>17</v>
       </c>
@@ -3521,7 +3523,7 @@
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16">
+    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
@@ -3544,7 +3546,7 @@
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="1:9" ht="16">
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>17</v>
       </c>
@@ -3567,7 +3569,7 @@
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
     </row>
-    <row r="18" spans="1:9" ht="16">
+    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
@@ -3590,7 +3592,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
     </row>
-    <row r="19" spans="1:9" ht="16">
+    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
@@ -3613,7 +3615,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" ht="16">
+    <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>17</v>
       </c>
@@ -3640,7 +3642,7 @@
       </c>
       <c r="I20" s="35"/>
     </row>
-    <row r="21" spans="1:9" ht="16">
+    <row r="21" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>17</v>
       </c>
@@ -3663,7 +3665,7 @@
       <c r="H21" s="35"/>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="1:9" ht="16">
+    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>17</v>
       </c>
@@ -3686,7 +3688,7 @@
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
     </row>
-    <row r="23" spans="1:9" ht="16">
+    <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
         <v>17</v>
       </c>
@@ -3709,7 +3711,7 @@
       <c r="H23" s="35"/>
       <c r="I23" s="35"/>
     </row>
-    <row r="24" spans="1:9" ht="16">
+    <row r="24" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
         <v>17</v>
       </c>
@@ -3750,25 +3752,25 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="41"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3785,7 +3787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3802,7 +3804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3811,7 +3813,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3828,7 +3830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3864,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>17</v>
       </c>
@@ -3879,7 +3881,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>17</v>
       </c>
@@ -3897,7 +3899,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
         <v>17</v>
       </c>
@@ -3933,26 +3935,26 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="9" customWidth="1"/>
+    <col min="3" max="4" width="15.125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="23.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="5" style="9" customWidth="1"/>
-    <col min="10" max="10" width="46.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="46.125" style="9" customWidth="1"/>
     <col min="11" max="11" width="31.5" style="9" customWidth="1"/>
     <col min="12" max="12" width="8" style="9" customWidth="1"/>
-    <col min="13" max="13" width="73.6640625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="73.625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="13.125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="20.625" style="8" customWidth="1"/>
     <col min="16" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4026,7 +4028,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
@@ -4100,7 +4102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
@@ -4156,7 +4158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
@@ -4197,7 +4199,7 @@
         <v>13</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>13</v>
@@ -4230,7 +4232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="17">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="24">
         <v>1001</v>
       </c>
@@ -4367,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="24">
         <v>1002</v>
       </c>
@@ -4427,7 +4429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="24">
         <v>1003</v>
       </c>
@@ -4492,7 +4494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="17">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="24">
         <v>1014</v>
       </c>
@@ -4554,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
         <v>100301</v>
       </c>
@@ -4624,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
         <v>100302</v>
       </c>
@@ -4684,7 +4686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="20" customFormat="1" ht="17">
+    <row r="12" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="26">
         <v>100303</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="24">
         <v>100001</v>
       </c>
@@ -4804,7 +4806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="24">
         <v>100002</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="24">
         <v>100003</v>
       </c>
@@ -4926,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="24">
         <v>100304</v>
       </c>
@@ -4986,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="17">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="24">
         <v>1013</v>
       </c>
@@ -5063,26 +5065,26 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="9" customWidth="1"/>
-    <col min="2" max="3" width="17.83203125" style="9" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="9" customWidth="1"/>
+    <col min="2" max="3" width="17.875" style="9" customWidth="1"/>
+    <col min="4" max="5" width="15.125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="19.875" style="9" customWidth="1"/>
     <col min="7" max="7" width="28" style="9" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="63.1640625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="23.125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16.125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="63.125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="20.125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="13.125" style="9" customWidth="1"/>
     <col min="14" max="14" width="9" style="9"/>
-    <col min="15" max="15" width="13.1640625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="9" customWidth="1"/>
     <col min="16" max="16" width="11" style="9" customWidth="1"/>
     <col min="17" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5150,7 +5152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -5218,7 +5220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -5269,7 +5271,7 @@
       </c>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -5338,7 +5340,7 @@
       </c>
       <c r="W4" s="12"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -5404,7 +5406,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <f t="shared" ref="A6:A16" si="0">200000+C6*100+D6</f>
         <v>200101</v>
@@ -5461,7 +5463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>200102</v>
@@ -5517,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>200103</v>
@@ -5576,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>200104</v>
@@ -5632,7 +5634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>200105</v>
@@ -5688,7 +5690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>200106</v>
@@ -5744,7 +5746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>200107</v>
@@ -5800,7 +5802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>200201</v>
@@ -5859,7 +5861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>200202</v>
@@ -5918,7 +5920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>200203</v>
@@ -5977,7 +5979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>200204</v>
@@ -6052,16 +6054,16 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="9" customWidth="1"/>
-    <col min="4" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="9" customWidth="1"/>
+    <col min="1" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="9" customWidth="1"/>
+    <col min="4" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="20.125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6090,7 +6092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6119,7 +6121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6140,7 +6142,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6169,7 +6171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -6198,7 +6200,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>177</v>
       </c>
@@ -6227,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>183</v>
       </c>
@@ -6256,7 +6258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>188</v>
       </c>
@@ -6285,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>193</v>
       </c>
@@ -6314,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -6325,7 +6327,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -6336,7 +6338,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -6347,7 +6349,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -6358,7 +6360,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -6369,7 +6371,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -6380,7 +6382,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -6391,7 +6393,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -6402,7 +6404,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -6413,7 +6415,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -6438,21 +6440,21 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="9" customWidth="1"/>
-    <col min="4" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" style="9" customWidth="1"/>
-    <col min="11" max="16377" width="17.1640625" customWidth="1"/>
+    <col min="1" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="9" customWidth="1"/>
+    <col min="4" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="9" width="25.625" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="9" customWidth="1"/>
+    <col min="11" max="16377" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6484,7 +6486,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6516,7 +6518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6538,7 +6540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6561,16 +6563,16 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -6602,7 +6604,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>200</v>
       </c>
@@ -6634,7 +6636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>202</v>
       </c>
@@ -6666,7 +6668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>206</v>
       </c>
@@ -6698,7 +6700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>210</v>
       </c>
@@ -6730,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -6742,7 +6744,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -6754,7 +6756,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -6766,7 +6768,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -6778,7 +6780,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -6790,19 +6792,19 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="10:10">
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="10:10">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="10:10">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J19" s="6"/>
     </row>
   </sheetData>
@@ -6820,18 +6822,18 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="35.625" customWidth="1"/>
+    <col min="10" max="10" width="21.875" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6869,7 +6871,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16">
+    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6907,7 +6909,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16">
+    <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6931,7 +6933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16">
+    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6969,7 +6971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16">
+    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -7007,7 +7009,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>215</v>
       </c>
@@ -7041,7 +7043,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>221</v>
       </c>
@@ -7075,7 +7077,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>226</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
+    <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>231</v>
       </c>

</xml_diff>

<commit_message>
use $ to get current cell value
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB5CD89-8AB6-3148-987F-0B4A6C468DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAAA6AB-38A7-CF4E-AF61-BE2B7A38F754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1870,9 +1870,6 @@
     <t>{200106}</t>
   </si>
   <si>
-    <t>value &gt; 0 &amp;&amp; value &lt; 20</t>
-  </si>
-  <si>
     <t>[1]</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1897,6 +1894,9 @@
   </si>
   <si>
     <t>key2=MAIN==#main.type&amp;condition=mainline_event</t>
+  </si>
+  <si>
+    <t>$ &gt; 0 &amp;&amp; $ &lt; 20</t>
   </si>
 </sst>
 </file>
@@ -3169,7 +3169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3185,7 +3185,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3283,7 +3283,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>13</v>
@@ -3769,7 +3769,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3937,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -4172,10 +4172,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -4205,7 +4205,7 @@
         <v>13</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>13</v>
@@ -6069,7 +6069,7 @@
     <col min="9" max="9" width="13.1640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.5">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -6460,7 +6460,7 @@
     <col min="11" max="16377" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6569,16 +6569,16 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.5">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
remove '!index' and '!key'
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE482087-28BF-A54C-9DB8-4D35A155316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68186292-A074-B04B-A2B6-FC43F57D1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1889,13 +1889,13 @@
     <t>#main.type=$&amp;key2=MAIN&amp;#main.condition=mainline_event</t>
   </si>
   <si>
-    <t>#define.value=$&amp;key1=TASK_TYPE</t>
-  </si>
-  <si>
     <t>item#item.id=$.id</t>
   </si>
   <si>
     <t>item#*.id=$.id</t>
+  </si>
+  <si>
+    <t>#define.value=$&amp;#define.key1=TASK_TYPE</t>
   </si>
 </sst>
 </file>
@@ -3936,7 +3936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4174,7 +4174,7 @@
         <v>257</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -6445,7 +6445,7 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -6568,10 +6568,10 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
refactor processor registration and enhance index checker functionality
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68186292-A074-B04B-A2B6-FC43F57D1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE6C439-CCEA-C948-96A3-D801C1C5A393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,7 +1101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="263">
   <si>
     <t>id</t>
   </si>
@@ -1886,16 +1886,19 @@
     <t>$ &gt; 0 &amp;&amp; $ &lt; 20</t>
   </si>
   <si>
-    <t>#main.type=$&amp;key2=MAIN&amp;#main.condition=mainline_event</t>
-  </si>
-  <si>
-    <t>item#item.id=$.id</t>
-  </si>
-  <si>
-    <t>item#*.id=$.id</t>
-  </si>
-  <si>
-    <t>#define.value=$&amp;#define.key1=TASK_TYPE</t>
+    <t>#define.value&amp;key1=TASK_TYPE</t>
+  </si>
+  <si>
+    <t>$&amp;key2=MAIN==#main.type&amp;condition=mainline_event</t>
+  </si>
+  <si>
+    <t>$[*].id==item#item.id</t>
+  </si>
+  <si>
+    <t>$[*].id==item#*.id</t>
+  </si>
+  <si>
+    <t>$[*]==#branch.id</t>
   </si>
 </sst>
 </file>
@@ -3282,7 +3285,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>13</v>
@@ -3937,7 +3940,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -4174,7 +4177,7 @@
         <v>257</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -4183,7 +4186,7 @@
         <v>101</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>102</v>
+        <v>262</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -6446,7 +6449,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16"/>
@@ -6568,10 +6571,10 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add array type support
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA8E83-8F5F-CC4B-80EC-264645E6E92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1877A711-5BFE-48BD-9D6A-58D78B4ACC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1101,7 +1101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="269">
   <si>
     <t>id</t>
   </si>
@@ -1386,9 +1386,6 @@
   </si>
   <si>
     <t>int?</t>
-  </si>
-  <si>
-    <t>table?</t>
   </si>
   <si>
     <t>bool?</t>
@@ -1862,12 +1859,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>{200105}</t>
-  </si>
-  <si>
-    <t>{200106}</t>
-  </si>
-  <si>
     <t>[1]</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1916,17 +1907,31 @@
   </si>
   <si>
     <t>参数类型</t>
+  </si>
+  <si>
+    <t>[200105]</t>
+  </si>
+  <si>
+    <t>[200106]</t>
+  </si>
+  <si>
+    <t>int[]?</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1955,7 +1960,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1975,7 +1980,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2128,7 +2133,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2193,12 +2198,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2261,7 +2260,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="常规 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
@@ -3192,150 +3191,150 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="45.875" customWidth="1"/>
+    <col min="6" max="6" width="18.625" customWidth="1"/>
+    <col min="8" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="42" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:9" ht="16">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16">
+      <c r="I2" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="G3" s="33" t="s">
+      <c r="F3" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16">
+      <c r="I3" s="32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-    </row>
-    <row r="5" spans="1:9" ht="16">
+      <c r="B4" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16">
+      <c r="B5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-    </row>
-    <row r="7" spans="1:9" ht="16">
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3353,18 +3352,18 @@
       <c r="G7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="35" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16">
+      <c r="I7" s="33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="11" t="s">
         <v>19</v>
       </c>
@@ -3380,14 +3379,14 @@
       <c r="G8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-    </row>
-    <row r="9" spans="1:9" ht="16">
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
@@ -3403,14 +3402,14 @@
       <c r="G9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" ht="16">
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
@@ -3426,14 +3425,14 @@
       <c r="G10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="1:9" ht="16">
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="11" t="s">
         <v>19</v>
       </c>
@@ -3449,14 +3448,14 @@
       <c r="G11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="1:9" ht="16">
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="11" t="s">
         <v>19</v>
       </c>
@@ -3472,14 +3471,14 @@
       <c r="G12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-    </row>
-    <row r="13" spans="1:9" ht="16">
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
@@ -3495,14 +3494,14 @@
       <c r="G13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9" ht="16">
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="33" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -3520,16 +3519,16 @@
       <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" ht="16">
+      <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="11" t="s">
         <v>37</v>
       </c>
@@ -3545,14 +3544,14 @@
       <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="16">
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
@@ -3568,14 +3567,14 @@
       <c r="G16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="1:9" ht="16">
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="11" t="s">
         <v>37</v>
       </c>
@@ -3591,14 +3590,14 @@
       <c r="G17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="1:9" ht="16">
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
@@ -3614,14 +3613,14 @@
       <c r="G18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="11" t="s">
         <v>37</v>
       </c>
@@ -3637,14 +3636,14 @@
       <c r="G19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="1:9" ht="16">
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="33" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -3662,16 +3661,16 @@
       <c r="G20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="35"/>
-    </row>
-    <row r="21" spans="1:9" ht="16">
+      <c r="I20" s="33"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="11" t="s">
         <v>60</v>
       </c>
@@ -3687,14 +3686,14 @@
       <c r="G21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="1:9" ht="16">
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="11" t="s">
         <v>60</v>
       </c>
@@ -3710,14 +3709,14 @@
       <c r="G22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" spans="1:9" ht="16">
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="11" t="s">
         <v>60</v>
       </c>
@@ -3733,31 +3732,31 @@
       <c r="G23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-    </row>
-    <row r="24" spans="1:9" ht="16">
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="35">
         <v>1023</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3777,30 +3776,30 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="41"/>
+    <col min="1" max="1" width="9" style="39"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="44" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -3812,7 +3811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3838,7 +3837,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3855,65 +3854,65 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>237</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="41" t="s">
+      <c r="C7" s="37">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" s="39">
-        <v>1200</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="40" t="s">
+      <c r="B8" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C8" s="39">
+      <c r="C8" s="37">
         <v>3</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="39">
+      <c r="C9" s="37">
         <f>7*3600</f>
         <v>25200</v>
       </c>
@@ -3921,17 +3920,17 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="39">
+      <c r="C10" s="37">
         <f>0.5*3600</f>
         <v>1800</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3956,30 +3955,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="9" customWidth="1"/>
+    <col min="3" max="4" width="15.125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="23.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="5" style="9" customWidth="1"/>
-    <col min="10" max="10" width="46.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="46.125" style="9" customWidth="1"/>
     <col min="11" max="11" width="31.5" style="9" customWidth="1"/>
     <col min="12" max="12" width="8" style="9" customWidth="1"/>
-    <col min="13" max="13" width="73.6640625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="73.625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="13.125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="20.625" style="8" customWidth="1"/>
     <col min="16" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3998,7 +3997,7 @@
       <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -4053,7 +4052,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -4072,26 +4071,26 @@
       <c r="F2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>95</v>
+      <c r="G2" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>94</v>
@@ -4127,7 +4126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
@@ -4138,19 +4137,19 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="22"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>13</v>
@@ -4183,7 +4182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
@@ -4191,19 +4190,19 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -4212,11 +4211,11 @@
         <v>13</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
@@ -4224,7 +4223,7 @@
         <v>13</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>13</v>
@@ -4257,84 +4256,84 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="S5" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="U5" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="W5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="X5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" s="22">
+        <v>1001</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="17">
-      <c r="A6" s="24">
-        <v>1001</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>122</v>
       </c>
       <c r="C6" s="15">
         <v>1</v>
@@ -4342,14 +4341,16 @@
       <c r="D6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>122</v>
+      <c r="E6" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="F6" s="15">
         <f t="shared" ref="F6:F16" si="0">A7</f>
         <v>1002</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="15" t="s">
+        <v>268</v>
+      </c>
       <c r="H6" s="16" t="s">
         <v>38</v>
       </c>
@@ -4357,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K6" s="15" t="str">
         <f>"{"&amp;O6&amp;"}"</f>
@@ -4366,8 +4367,8 @@
       <c r="L6" s="15">
         <v>0</v>
       </c>
-      <c r="M6" s="29" t="s">
-        <v>124</v>
+      <c r="M6" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="N6" s="9">
         <v>1</v>
@@ -4394,12 +4395,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="22">
         <v>1002</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>125</v>
+      <c r="B7" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="15">
         <v>2</v>
@@ -4407,14 +4408,14 @@
       <c r="D7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>125</v>
+      <c r="E7" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="F7" s="15">
         <f t="shared" si="0"/>
         <v>1003</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="9" t="s">
         <v>38</v>
       </c>
@@ -4422,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" s="15" t="str">
         <f t="shared" ref="K7:K9" si="1">"{"&amp;O7&amp;"}"</f>
@@ -4454,12 +4455,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17">
-      <c r="A8" s="24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
         <v>1003</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>127</v>
+      <c r="B8" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="C8" s="15">
         <v>3</v>
@@ -4467,8 +4468,8 @@
       <c r="D8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>127</v>
+      <c r="E8" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="F8" s="15">
         <f t="shared" si="0"/>
@@ -4481,7 +4482,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K8" s="15" t="str">
         <f t="shared" si="1"/>
@@ -4519,12 +4520,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="17">
-      <c r="A9" s="24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" s="22">
         <v>1014</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>129</v>
+      <c r="B9" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="C9" s="15">
         <v>4</v>
@@ -4532,15 +4533,15 @@
       <c r="D9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>129</v>
+      <c r="E9" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="F9" s="15">
         <f t="shared" si="0"/>
         <v>100301</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>251</v>
+      <c r="G9" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>57</v>
@@ -4581,12 +4582,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
-      <c r="A10" s="24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" s="22">
         <v>100301</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>130</v>
+      <c r="B10" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="C10" s="15">
         <v>5</v>
@@ -4594,15 +4595,15 @@
       <c r="D10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>130</v>
+      <c r="E10" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="F10" s="15">
         <f t="shared" si="0"/>
         <v>100302</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>252</v>
+      <c r="G10" s="15" t="s">
+        <v>266</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>38</v>
@@ -4611,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K10" s="15" t="str">
         <f t="shared" ref="K10:K11" si="3">"{"&amp;O10&amp;"}"</f>
@@ -4620,8 +4621,8 @@
       <c r="L10" s="15">
         <v>0</v>
       </c>
-      <c r="M10" s="29" t="s">
-        <v>132</v>
+      <c r="M10" s="27" t="s">
+        <v>131</v>
       </c>
       <c r="N10" s="9">
         <v>1</v>
@@ -4651,12 +4652,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17">
-      <c r="A11" s="24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" s="22">
         <v>100302</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>133</v>
+      <c r="B11" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="C11" s="15">
         <v>6</v>
@@ -4664,14 +4665,14 @@
       <c r="D11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>133</v>
+      <c r="E11" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="F11" s="15">
         <f t="shared" si="0"/>
         <v>100303</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="16" t="s">
         <v>38</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K11" s="15" t="str">
         <f t="shared" si="3"/>
@@ -4711,48 +4712,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="20" customFormat="1" ht="17">
-      <c r="A12" s="26">
+    <row r="12" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24">
         <v>100303</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>135</v>
+      <c r="B12" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C12" s="15">
         <v>7</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>135</v>
+      <c r="E12" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="F12" s="15">
         <f t="shared" si="0"/>
         <v>100001</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="26">
         <v>1</v>
       </c>
-      <c r="J12" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="K12" s="27" t="str">
+      <c r="J12" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="K12" s="25" t="str">
         <f t="shared" ref="K12:K17" si="5">"{"&amp;O12&amp;"}"</f>
         <v>{{10201,10}}</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="25">
         <v>0</v>
       </c>
-      <c r="M12" s="27"/>
+      <c r="M12" s="25"/>
       <c r="N12" s="20">
         <v>1</v>
       </c>
-      <c r="O12" s="32" t="str">
+      <c r="O12" s="30" t="str">
         <f t="shared" ref="O12:O17" si="6">IF(P12="","","{"&amp;P12&amp;","&amp;Q12&amp;"}")&amp;IF(R12="","",",{"&amp;R12&amp;","&amp;S12&amp;"}")&amp;IF(T12="","",",{"&amp;T12&amp;","&amp;U12&amp;"}")</f>
         <v>{10201,10}</v>
       </c>
@@ -4771,12 +4772,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17">
-      <c r="A13" s="24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" s="22">
         <v>100001</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>137</v>
+      <c r="B13" s="23" t="s">
+        <v>136</v>
       </c>
       <c r="C13" s="15">
         <v>8</v>
@@ -4784,14 +4785,14 @@
       <c r="D13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>137</v>
+      <c r="E13" s="23" t="s">
+        <v>136</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" si="0"/>
         <v>100002</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="16" t="s">
         <v>38</v>
       </c>
@@ -4799,7 +4800,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K13" s="15" t="str">
         <f t="shared" ref="K13:K14" si="7">"{"&amp;O13&amp;"}"</f>
@@ -4831,12 +4832,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
-      <c r="A14" s="24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" s="22">
         <v>100002</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>139</v>
+      <c r="B14" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="C14" s="15">
         <v>9</v>
@@ -4844,14 +4845,14 @@
       <c r="D14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>139</v>
+      <c r="E14" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="F14" s="15">
         <f t="shared" si="0"/>
         <v>100003</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="9" t="s">
         <v>38</v>
       </c>
@@ -4859,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K14" s="15" t="str">
         <f t="shared" si="7"/>
@@ -4891,12 +4892,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
-      <c r="A15" s="24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" s="22">
         <v>100003</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>141</v>
+      <c r="B15" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="C15" s="15">
         <v>10</v>
@@ -4904,14 +4905,14 @@
       <c r="D15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="25" t="s">
-        <v>141</v>
+      <c r="E15" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="F15" s="15">
         <f t="shared" si="0"/>
         <v>100304</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="9" t="s">
         <v>38</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K15" s="15" t="str">
         <f t="shared" ref="K15" si="9">"{"&amp;O15&amp;"}"</f>
@@ -4928,8 +4929,8 @@
       <c r="L15" s="15">
         <v>0</v>
       </c>
-      <c r="M15" s="29" t="s">
-        <v>143</v>
+      <c r="M15" s="27" t="s">
+        <v>142</v>
       </c>
       <c r="N15" s="9">
         <v>1</v>
@@ -4953,12 +4954,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17">
-      <c r="A16" s="24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
         <v>100304</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>144</v>
+      <c r="B16" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="C16" s="15">
         <v>11</v>
@@ -4966,14 +4967,14 @@
       <c r="D16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="25" t="s">
-        <v>144</v>
+      <c r="E16" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="F16" s="15">
         <f t="shared" si="0"/>
         <v>1013</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="16" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K16" s="15" t="str">
         <f t="shared" si="5"/>
@@ -5013,12 +5014,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="17">
-      <c r="A17" s="24">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="22">
         <v>1013</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>146</v>
+      <c r="B17" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="C17" s="15">
         <v>12</v>
@@ -5026,11 +5027,11 @@
       <c r="D17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>146</v>
+      <c r="E17" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="16" t="s">
         <v>54</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K17" s="15" t="str">
         <f t="shared" si="5"/>
@@ -5086,31 +5087,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="9" customWidth="1"/>
-    <col min="2" max="3" width="17.83203125" style="9" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="9" customWidth="1"/>
+    <col min="2" max="3" width="17.875" style="9" customWidth="1"/>
+    <col min="4" max="5" width="15.125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="19.875" style="9" customWidth="1"/>
     <col min="7" max="7" width="28" style="9" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="63.1640625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="23.125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16.125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="63.125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="8.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="13.125" style="9" customWidth="1"/>
     <col min="15" max="15" width="9" style="9"/>
-    <col min="16" max="16" width="13.1640625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="13.125" style="9" customWidth="1"/>
     <col min="17" max="17" width="11" style="9" customWidth="1"/>
     <col min="18" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5118,7 +5119,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>73</v>
@@ -5127,7 +5128,7 @@
         <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>75</v>
@@ -5145,7 +5146,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>80</v>
@@ -5181,7 +5182,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -5210,16 +5211,16 @@
         <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>11</v>
@@ -5252,7 +5253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -5263,7 +5264,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -5273,13 +5274,13 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>13</v>
@@ -5304,7 +5305,7 @@
       </c>
       <c r="X3" s="1"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
@@ -5342,7 +5343,7 @@
         <v>13</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
@@ -5376,82 +5377,82 @@
       </c>
       <c r="X4" s="12"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="R5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="U5" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>118</v>
-      </c>
       <c r="W5" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <f t="shared" ref="A6:A16" si="0">200000+C6*100+D6</f>
         <v>200101</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6">
         <f>COUNTIF($D$6:D6,1)</f>
@@ -5464,7 +5465,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="6" t="str">
         <f>"支线·"&amp;F6</f>
@@ -5478,10 +5479,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M6" s="15" t="str">
         <f t="shared" ref="M6:M16" si="1">"{"&amp;Q6&amp;"}"</f>
@@ -5505,13 +5506,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>200102</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -5523,7 +5524,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7" s="6" t="str">
         <f t="shared" ref="G7:G16" si="3">"支线·"&amp;F7</f>
@@ -5540,7 +5541,7 @@
         <v>53</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M7" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5564,13 +5565,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>200103</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -5582,7 +5583,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5599,10 +5600,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M8" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5626,13 +5627,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>200104</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -5644,7 +5645,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G9" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5658,10 +5659,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M9" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5685,13 +5686,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>200105</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -5703,7 +5704,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G10" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5717,10 +5718,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M10" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5744,13 +5745,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>200106</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
@@ -5762,7 +5763,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G11" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5776,10 +5777,10 @@
         <v>0</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M11" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5803,13 +5804,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>200107</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -5821,7 +5822,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G12" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5835,10 +5836,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M12" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5862,13 +5863,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>200201</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
@@ -5880,7 +5881,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G13" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5897,10 +5898,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M13" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5924,13 +5925,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>200202</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -5942,7 +5943,7 @@
         <v>24</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" s="6" t="str">
         <f t="shared" si="3"/>
@@ -5959,10 +5960,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M14" s="15" t="str">
         <f t="shared" si="1"/>
@@ -5986,13 +5987,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>200203</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
@@ -6004,7 +6005,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="6" t="str">
         <f t="shared" si="3"/>
@@ -6021,10 +6022,10 @@
         <v>0</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M15" s="15" t="str">
         <f t="shared" si="1"/>
@@ -6048,13 +6049,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>200204</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="6">
         <v>2</v>
@@ -6066,7 +6067,7 @@
         <v>24</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G16" s="6" t="str">
         <f t="shared" si="3"/>
@@ -6080,10 +6081,10 @@
         <v>0</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M16" s="15" t="str">
         <f t="shared" si="1"/>
@@ -6126,16 +6127,16 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="9" customWidth="1"/>
-    <col min="4" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="9" customWidth="1"/>
+    <col min="1" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="9" customWidth="1"/>
+    <col min="4" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="20.125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6164,7 +6165,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6184,16 +6185,16 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6204,17 +6205,17 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6237,47 +6238,47 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -6286,27 +6287,27 @@
         <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -6315,27 +6316,27 @@
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="C8" s="6">
         <v>3</v>
@@ -6344,27 +6345,27 @@
         <v>4</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="C9" s="6">
         <v>4</v>
@@ -6373,22 +6374,22 @@
         <v>4</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="I9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -6399,7 +6400,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -6410,7 +6411,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -6421,7 +6422,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -6432,7 +6433,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -6443,7 +6444,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -6454,7 +6455,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -6465,7 +6466,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -6476,7 +6477,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -6487,7 +6488,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -6516,17 +6517,17 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="9" customWidth="1"/>
-    <col min="4" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" style="9" customWidth="1"/>
-    <col min="11" max="16377" width="17.1640625" customWidth="1"/>
+    <col min="1" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="9" customWidth="1"/>
+    <col min="4" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="9" width="25.625" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="9" customWidth="1"/>
+    <col min="11" max="16377" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6552,13 +6553,13 @@
         <v>80</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6578,19 +6579,19 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6601,18 +6602,18 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -6635,53 +6636,53 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -6699,21 +6700,21 @@
         <v>45</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J6" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -6722,30 +6723,30 @@
         <v>5</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="C8" s="6">
         <v>3</v>
@@ -6754,30 +6755,30 @@
         <v>5</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="C9" s="6">
         <v>4</v>
@@ -6786,25 +6787,25 @@
         <v>5</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -6816,7 +6817,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -6828,7 +6829,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -6840,7 +6841,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -6852,7 +6853,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -6864,19 +6865,19 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="10:10">
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="10:10">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="10:10">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J19" s="6"/>
     </row>
   </sheetData>
@@ -6894,18 +6895,18 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="35.625" customWidth="1"/>
+    <col min="10" max="10" width="21.875" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6943,7 +6944,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16">
+    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -6966,22 +6967,22 @@
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -6993,19 +6994,19 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -7022,7 +7023,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -7034,7 +7035,7 @@
         <v>13</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>13</v>
@@ -7043,50 +7044,50 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16">
+    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="L5" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
@@ -7095,7 +7096,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
@@ -7103,24 +7104,24 @@
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
       </c>
       <c r="L6" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="C7" s="6">
         <v>3</v>
@@ -7129,7 +7130,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
@@ -7137,24 +7138,24 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
       </c>
       <c r="L7" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="16">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="C8" s="6">
         <v>4</v>
@@ -7163,7 +7164,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
@@ -7171,24 +7172,24 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
       </c>
       <c r="L8" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="4" t="s">
-        <v>230</v>
-      </c>
       <c r="B9" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="6">
         <v>5</v>
@@ -7197,7 +7198,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
@@ -7205,16 +7206,16 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K9" s="6">
         <v>0</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convert value in indexer filter
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1877A711-5BFE-48BD-9D6A-58D78B4ACC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F93D561-9D48-44CC-A724-6B5D31344B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-15" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1101,7 +1101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="270">
   <si>
     <t>id</t>
   </si>
@@ -1920,6 +1920,10 @@
   </si>
   <si>
     <t>[]</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>task#*.id&amp;type=MAIN</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -3188,7 +3192,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3956,7 +3960,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -3965,7 +3969,7 @@
     <col min="2" max="2" width="17.875" style="9" customWidth="1"/>
     <col min="3" max="4" width="15.125" style="9" customWidth="1"/>
     <col min="5" max="5" width="26.875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.75" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.125" style="9" customWidth="1"/>
     <col min="8" max="8" width="23.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="5" style="9" customWidth="1"/>
@@ -4199,7 +4203,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
+        <v>269</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>258</v>

</xml_diff>

<commit_message>
add example for stringify rule
</commit_message>
<xml_diff>
--- a/test/res/task.xlsx
+++ b/test/res/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F93D561-9D48-44CC-A724-6B5D31344B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718CF2AC-EFC2-455B-8CF6-1B8D933B94F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-15" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32100" yWindow="1425" windowWidth="28395" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="9" r:id="rId1"/>
@@ -1863,10 +1863,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>@define</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>@config</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1924,6 +1920,10 @@
   </si>
   <si>
     <t>task#*.id&amp;type=MAIN</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>@define;@stringify(task)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -3191,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3207,7 +3207,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -3261,7 +3261,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>11</v>
@@ -3305,7 +3305,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>13</v>
@@ -3791,7 +3791,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3959,7 +3959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -4067,7 +4067,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -4076,7 +4076,7 @@
         <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>11</v>
@@ -4194,19 +4194,19 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -4353,7 +4353,7 @@
         <v>1002</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>38</v>
@@ -4545,7 +4545,7 @@
         <v>100301</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>57</v>
@@ -4607,7 +4607,7 @@
         <v>100302</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>38</v>
@@ -5150,7 +5150,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>80</v>
@@ -5200,7 +5200,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -5218,7 +5218,7 @@
         <v>95</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>11</v>
@@ -5347,7 +5347,7 @@
         <v>13</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
@@ -5416,7 +5416,7 @@
         <v>109</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>110</v>
@@ -6640,10 +6640,10 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>

</xml_diff>